<commit_message>
Removed finally covered holes.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_uncovered_coverage_explanation.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_uncovered_coverage_explanation.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/OpenHW Group/RTL_freeze_v2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1699" documentId="8_{F34CC886-E7E9-45AE-87EF-35A6981A753F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE28892F-4659-4E84-BC03-7E83001AE0DE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7927129-0A1A-41BB-BC08-DF3237CB7F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="789" xr2:uid="{9C133A6F-F4C2-4C35-A1E6-85F78A61AE65}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="789" xr2:uid="{9C133A6F-F4C2-4C35-A1E6-85F78A61AE65}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Cov uncovered (CFG_P)" sheetId="4" r:id="rId1"/>
     <sheet name="Code Cov uncovered (CFG_P_F0)" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Code Cov uncovered (CFG_P)'!$A$1:$U$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Code Cov uncovered (CFG_P)'!$A$1:$T$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Code Cov uncovered (CFG_P_F0)'!$A$1:$U$2</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>CFG_P</t>
   </si>
@@ -110,71 +110,7 @@
 Inside DECODE_HWLOOP state.</t>
   </si>
   <si>
-    <t>Need assertion proof</t>
-  </si>
-  <si>
-    <t>I do not understand the comment: "we can be at the end of HWloop due to a return from interrupt or ...". Does this mean, a return-from-exception into the last instruction of HWLoop1?</t>
-  </si>
-  <si>
-    <t>I have performed a reachability analysis of these conditions for the cv32e40p_controller module and in that context these are reachable conditions.  However, a proper analysis should entail the full id_stage (or perhaps even the entire core).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">could add test? Complicated. </t>
-  </si>
-  <si>
-    <t>missing test for condition row4:
-trigger match on an ebreak where ebreakm is 0.</t>
-  </si>
-  <si>
     <t>related to HWLOOP only</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">No trigger match without ebrk_force_debug_mode???
-No ebreak execution without ebreakm set in DCSR?
-What is the behavior when ebreakm is 0? (not in spec)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>condition row 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (trigger_match_i_1) TBD
-row4 hole: trigger_match_i == 1 when (~debug_req_entry_q &amp;&amp; ~data_load_event_i &amp;&amp; ~(ebrk_force_debug_mode &amp;&amp; ebrk_insn_i) &amp;&amp; ~debug_mode_q)
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>row 4 should be covered with a trigger match on an ebreak where ebreakm is 0.
-Tried to prove using Siemens EDA QuestaFormal but</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF9C5700"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> row4 condition inconclusive.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -192,12 +128,20 @@
       <t>for cv32e40p_controller)</t>
     </r>
   </si>
+  <si>
+    <t>Need assertion proof
+Could be proven with JasperGold?</t>
+  </si>
+  <si>
+    <t>Could add test?
+Could be proven with JasperGold?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,14 +173,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,38 +236,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -649,96 +585,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C3E37B-E87C-4EDB-8A44-82012E83B017}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
-    <col min="2" max="7" width="6.44140625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="6.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.44140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="28.5546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="54.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30" style="1" customWidth="1"/>
+    <col min="12" max="12" width="34.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.88671875" style="6" customWidth="1"/>
-    <col min="14" max="14" width="35.88671875" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="3"/>
+    <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="9">
         <v>831</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -747,158 +680,121 @@
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="9">
         <v>852</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="9">
         <v>850</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="9">
         <v>850</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="9">
         <v>867</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="9">
         <v>872</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="9">
         <v>865</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="9">
         <v>870</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J5" s="13"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="9">
         <v>877</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="9">
         <v>882</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="9">
         <v>875</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="9">
         <v>880</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="13"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="9">
         <v>887</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="9">
         <v>885</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="10"/>
-    </row>
-    <row r="8" spans="1:15" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="17">
-        <v>1241</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U8" xr:uid="{A3C3E37B-E87C-4EDB-8A44-82012E83B017}">
+  <autoFilter ref="A1:T7" xr:uid="{A3C3E37B-E87C-4EDB-8A44-82012E83B017}">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
-  <mergeCells count="17">
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="K4:K7"/>
+  <mergeCells count="15">
     <mergeCell ref="J4:J7"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -909,6 +805,11 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="K4:K7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -942,340 +843,340 @@
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="B3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U2" xr:uid="{A3C3E37B-E87C-4EDB-8A44-82012E83B017}">
@@ -1304,14 +1205,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1564,27 +1463,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72DFD955-914C-4D26-8F31-FE203C0485CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCBB5CA-1E73-4C95-B488-5F0C07035068}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1609,9 +1501,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCBB5CA-1E73-4C95-B488-5F0C07035068}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72DFD955-914C-4D26-8F31-FE203C0485CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>